<commit_message>
Workflow Name : TC_01.xaml, TC_02.xaml Description : Added Object Repository Date : Jagannath Patil Developer Name : Jagannath Patil
</commit_message>
<xml_diff>
--- a/Data/Input/TestCases.xlsx
+++ b/Data/Input/TestCases.xlsx
@@ -2853,13 +2853,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2880,26 +2889,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3130,10 +3130,10 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F7" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="2" spans="1:12" s="10" customFormat="1" ht="45">
       <c r="A2" s="41" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>298</v>
@@ -4163,16 +4163,16 @@
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" s="18" customFormat="1" ht="45">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="51" t="s">
         <v>321</v>
       </c>
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="51" t="s">
         <v>321</v>
       </c>
-      <c r="D18" s="59" t="s">
+      <c r="D18" s="53" t="s">
         <v>640</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -4199,10 +4199,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A19" s="63"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="60"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="54"/>
       <c r="E19" s="3" t="s">
         <v>13</v>
       </c>
@@ -4225,10 +4225,10 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A20" s="63"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="60"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="3" t="s">
         <v>14</v>
       </c>
@@ -4251,10 +4251,10 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" s="10" customFormat="1" ht="60">
-      <c r="A21" s="63"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="60"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="3" t="s">
         <v>15</v>
       </c>
@@ -4279,10 +4279,10 @@
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A22" s="63"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="60"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="3" t="s">
         <v>16</v>
       </c>
@@ -4305,10 +4305,10 @@
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" s="10" customFormat="1" ht="25.5">
-      <c r="A23" s="63"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="60"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="3" t="s">
         <v>17</v>
       </c>
@@ -4333,10 +4333,10 @@
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" s="10" customFormat="1" ht="25.5">
-      <c r="A24" s="63"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="60"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="54"/>
       <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
@@ -4361,10 +4361,10 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A25" s="63"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="60"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="54"/>
       <c r="E25" s="3" t="s">
         <v>19</v>
       </c>
@@ -4389,10 +4389,10 @@
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A26" s="63"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="60"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="54"/>
       <c r="E26" s="3" t="s">
         <v>20</v>
       </c>
@@ -4417,10 +4417,10 @@
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A27" s="63"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="60"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="3" t="s">
         <v>21</v>
       </c>
@@ -4443,10 +4443,10 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A28" s="63"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="60"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="54"/>
       <c r="E28" s="3" t="s">
         <v>22</v>
       </c>
@@ -4471,10 +4471,10 @@
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A29" s="63"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="60"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="3" t="s">
         <v>23</v>
       </c>
@@ -4497,10 +4497,10 @@
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A30" s="63"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="61"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="3" t="s">
         <v>24</v>
       </c>
@@ -4973,16 +4973,16 @@
       <c r="L46" s="19"/>
     </row>
     <row r="47" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="D47" s="53" t="s">
         <v>640</v>
       </c>
       <c r="E47" s="37" t="s">
@@ -5009,10 +5009,10 @@
       <c r="L47" s="6"/>
     </row>
     <row r="48" spans="1:12" s="10" customFormat="1" ht="30">
-      <c r="A48" s="54"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="60"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="54"/>
       <c r="E48" s="37" t="s">
         <v>13</v>
       </c>
@@ -5035,10 +5035,10 @@
       <c r="L48" s="6"/>
     </row>
     <row r="49" spans="1:12" s="10" customFormat="1" ht="30">
-      <c r="A49" s="54"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="60"/>
+      <c r="A49" s="57"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="54"/>
       <c r="E49" s="37" t="s">
         <v>14</v>
       </c>
@@ -5063,10 +5063,10 @@
       <c r="L49" s="6"/>
     </row>
     <row r="50" spans="1:12" s="10" customFormat="1" ht="60">
-      <c r="A50" s="54"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="60"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="54"/>
       <c r="E50" s="37" t="s">
         <v>15</v>
       </c>
@@ -5091,10 +5091,10 @@
       <c r="L50" s="6"/>
     </row>
     <row r="51" spans="1:12" s="10" customFormat="1" ht="60">
-      <c r="A51" s="54"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="60"/>
+      <c r="A51" s="57"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="54"/>
       <c r="E51" s="37" t="s">
         <v>16</v>
       </c>
@@ -5119,10 +5119,10 @@
       <c r="L51" s="6"/>
     </row>
     <row r="52" spans="1:12" s="10" customFormat="1" ht="75">
-      <c r="A52" s="54"/>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="60"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="54"/>
       <c r="E52" s="37" t="s">
         <v>17</v>
       </c>
@@ -5147,10 +5147,10 @@
       <c r="L52" s="6"/>
     </row>
     <row r="53" spans="1:12" s="10" customFormat="1" ht="75">
-      <c r="A53" s="54"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="60"/>
+      <c r="A53" s="57"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="54"/>
       <c r="E53" s="37" t="s">
         <v>18</v>
       </c>
@@ -5175,10 +5175,10 @@
       <c r="L53" s="6"/>
     </row>
     <row r="54" spans="1:12" s="10" customFormat="1" ht="60">
-      <c r="A54" s="54"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="60"/>
+      <c r="A54" s="57"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="54"/>
       <c r="E54" s="37" t="s">
         <v>19</v>
       </c>
@@ -5203,10 +5203,10 @@
       <c r="L54" s="6"/>
     </row>
     <row r="55" spans="1:12" s="10" customFormat="1" ht="75">
-      <c r="A55" s="54"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="60"/>
+      <c r="A55" s="57"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="54"/>
       <c r="E55" s="37" t="s">
         <v>20</v>
       </c>
@@ -5231,10 +5231,10 @@
       <c r="L55" s="6"/>
     </row>
     <row r="56" spans="1:12" s="10" customFormat="1" ht="75">
-      <c r="A56" s="54"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="60"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="54"/>
       <c r="E56" s="37" t="s">
         <v>21</v>
       </c>
@@ -5259,10 +5259,10 @@
       <c r="L56" s="6"/>
     </row>
     <row r="57" spans="1:12" s="10" customFormat="1" ht="30">
-      <c r="A57" s="54"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="60"/>
+      <c r="A57" s="57"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="54"/>
       <c r="E57" s="37" t="s">
         <v>22</v>
       </c>
@@ -5287,10 +5287,10 @@
       <c r="L57" s="6"/>
     </row>
     <row r="58" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A58" s="55"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="61"/>
+      <c r="A58" s="58"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="55"/>
       <c r="E58" s="37" t="s">
         <v>23</v>
       </c>
@@ -5313,7 +5313,7 @@
       <c r="L58" s="6"/>
     </row>
     <row r="59" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A59" s="50" t="s">
+      <c r="A59" s="62" t="s">
         <v>78</v>
       </c>
       <c r="B59" s="44" t="s">
@@ -5349,7 +5349,7 @@
       <c r="L59" s="19"/>
     </row>
     <row r="60" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A60" s="51"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="45"/>
       <c r="C60" s="45"/>
       <c r="D60" s="48"/>
@@ -5375,7 +5375,7 @@
       <c r="L60" s="19"/>
     </row>
     <row r="61" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A61" s="51"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="45"/>
       <c r="C61" s="45"/>
       <c r="D61" s="48"/>
@@ -5401,7 +5401,7 @@
       <c r="L61" s="19"/>
     </row>
     <row r="62" spans="1:12" s="10" customFormat="1" ht="45">
-      <c r="A62" s="51"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
       <c r="D62" s="48"/>
@@ -5427,7 +5427,7 @@
       <c r="L62" s="19"/>
     </row>
     <row r="63" spans="1:12" s="10" customFormat="1" ht="60">
-      <c r="A63" s="51"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="45"/>
       <c r="C63" s="45"/>
       <c r="D63" s="48"/>
@@ -5453,7 +5453,7 @@
       <c r="L63" s="19"/>
     </row>
     <row r="64" spans="1:12" s="10" customFormat="1" ht="60">
-      <c r="A64" s="51"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="45"/>
       <c r="C64" s="45"/>
       <c r="D64" s="48"/>
@@ -5479,7 +5479,7 @@
       <c r="L64" s="19"/>
     </row>
     <row r="65" spans="1:12" s="10" customFormat="1" ht="38.25">
-      <c r="A65" s="52"/>
+      <c r="A65" s="64"/>
       <c r="B65" s="46"/>
       <c r="C65" s="46"/>
       <c r="D65" s="49"/>
@@ -5505,16 +5505,16 @@
       <c r="L65" s="19"/>
     </row>
     <row r="66" spans="1:12" ht="45">
-      <c r="A66" s="53" t="s">
+      <c r="A66" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="62" t="s">
+      <c r="C66" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="D66" s="59" t="s">
+      <c r="D66" s="53" t="s">
         <v>640</v>
       </c>
       <c r="E66" s="26" t="s">
@@ -5541,10 +5541,10 @@
       <c r="L66" s="6"/>
     </row>
     <row r="67" spans="1:12" ht="30">
-      <c r="A67" s="54"/>
-      <c r="B67" s="57"/>
-      <c r="C67" s="60"/>
-      <c r="D67" s="60"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="54"/>
       <c r="E67" s="26" t="s">
         <v>13</v>
       </c>
@@ -5567,10 +5567,10 @@
       <c r="L67" s="6"/>
     </row>
     <row r="68" spans="1:12" ht="45">
-      <c r="A68" s="54"/>
-      <c r="B68" s="57"/>
-      <c r="C68" s="60"/>
-      <c r="D68" s="60"/>
+      <c r="A68" s="57"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
       <c r="E68" s="26" t="s">
         <v>14</v>
       </c>
@@ -5595,10 +5595,10 @@
       <c r="L68" s="6"/>
     </row>
     <row r="69" spans="1:12" ht="45">
-      <c r="A69" s="54"/>
-      <c r="B69" s="57"/>
-      <c r="C69" s="60"/>
-      <c r="D69" s="60"/>
+      <c r="A69" s="57"/>
+      <c r="B69" s="60"/>
+      <c r="C69" s="54"/>
+      <c r="D69" s="54"/>
       <c r="E69" s="26" t="s">
         <v>15</v>
       </c>
@@ -5623,10 +5623,10 @@
       <c r="L69" s="6"/>
     </row>
     <row r="70" spans="1:12" ht="60">
-      <c r="A70" s="54"/>
-      <c r="B70" s="57"/>
-      <c r="C70" s="60"/>
-      <c r="D70" s="60"/>
+      <c r="A70" s="57"/>
+      <c r="B70" s="60"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
       <c r="E70" s="26" t="s">
         <v>16</v>
       </c>
@@ -5651,10 +5651,10 @@
       <c r="L70" s="6"/>
     </row>
     <row r="71" spans="1:12" ht="45">
-      <c r="A71" s="54"/>
-      <c r="B71" s="57"/>
-      <c r="C71" s="60"/>
-      <c r="D71" s="60"/>
+      <c r="A71" s="57"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
       <c r="E71" s="26" t="s">
         <v>17</v>
       </c>
@@ -5679,10 +5679,10 @@
       <c r="L71" s="6"/>
     </row>
     <row r="72" spans="1:12" ht="45">
-      <c r="A72" s="54"/>
-      <c r="B72" s="57"/>
-      <c r="C72" s="60"/>
-      <c r="D72" s="60"/>
+      <c r="A72" s="57"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
       <c r="E72" s="26" t="s">
         <v>18</v>
       </c>
@@ -5707,10 +5707,10 @@
       <c r="L72" s="6"/>
     </row>
     <row r="73" spans="1:12" ht="30">
-      <c r="A73" s="54"/>
-      <c r="B73" s="57"/>
-      <c r="C73" s="60"/>
-      <c r="D73" s="60"/>
+      <c r="A73" s="57"/>
+      <c r="B73" s="60"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
       <c r="E73" s="26" t="s">
         <v>19</v>
       </c>
@@ -5735,10 +5735,10 @@
       <c r="L73" s="24"/>
     </row>
     <row r="74" spans="1:12" ht="30">
-      <c r="A74" s="54"/>
-      <c r="B74" s="57"/>
-      <c r="C74" s="60"/>
-      <c r="D74" s="60"/>
+      <c r="A74" s="57"/>
+      <c r="B74" s="60"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="54"/>
       <c r="E74" s="26" t="s">
         <v>20</v>
       </c>
@@ -5763,10 +5763,10 @@
       <c r="L74" s="24"/>
     </row>
     <row r="75" spans="1:12" ht="45">
-      <c r="A75" s="54"/>
-      <c r="B75" s="57"/>
-      <c r="C75" s="60"/>
-      <c r="D75" s="60"/>
+      <c r="A75" s="57"/>
+      <c r="B75" s="60"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
       <c r="E75" s="26" t="s">
         <v>21</v>
       </c>
@@ -5789,10 +5789,10 @@
       <c r="L75" s="24"/>
     </row>
     <row r="76" spans="1:12" ht="38.25">
-      <c r="A76" s="55"/>
-      <c r="B76" s="58"/>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
+      <c r="A76" s="58"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="55"/>
       <c r="E76" s="26" t="s">
         <v>22</v>
       </c>
@@ -5815,7 +5815,7 @@
       <c r="L76" s="24"/>
     </row>
     <row r="77" spans="1:12" ht="45">
-      <c r="A77" s="50" t="s">
+      <c r="A77" s="62" t="s">
         <v>148</v>
       </c>
       <c r="B77" s="44" t="s">
@@ -5851,7 +5851,7 @@
       <c r="L77" s="19"/>
     </row>
     <row r="78" spans="1:12" ht="30">
-      <c r="A78" s="51"/>
+      <c r="A78" s="63"/>
       <c r="B78" s="45"/>
       <c r="C78" s="45"/>
       <c r="D78" s="48"/>
@@ -5877,7 +5877,7 @@
       <c r="L78" s="19"/>
     </row>
     <row r="79" spans="1:12" ht="30">
-      <c r="A79" s="51"/>
+      <c r="A79" s="63"/>
       <c r="B79" s="45"/>
       <c r="C79" s="45"/>
       <c r="D79" s="48"/>
@@ -5905,7 +5905,7 @@
       <c r="L79" s="19"/>
     </row>
     <row r="80" spans="1:12" ht="30">
-      <c r="A80" s="51"/>
+      <c r="A80" s="63"/>
       <c r="B80" s="45"/>
       <c r="C80" s="45"/>
       <c r="D80" s="48"/>
@@ -5933,7 +5933,7 @@
       <c r="L80" s="19"/>
     </row>
     <row r="81" spans="1:12" ht="30">
-      <c r="A81" s="51"/>
+      <c r="A81" s="63"/>
       <c r="B81" s="45"/>
       <c r="C81" s="45"/>
       <c r="D81" s="48"/>
@@ -5961,7 +5961,7 @@
       <c r="L81" s="19"/>
     </row>
     <row r="82" spans="1:12" ht="30">
-      <c r="A82" s="51"/>
+      <c r="A82" s="63"/>
       <c r="B82" s="45"/>
       <c r="C82" s="45"/>
       <c r="D82" s="48"/>
@@ -5989,7 +5989,7 @@
       <c r="L82" s="19"/>
     </row>
     <row r="83" spans="1:12" ht="45">
-      <c r="A83" s="51"/>
+      <c r="A83" s="63"/>
       <c r="B83" s="45"/>
       <c r="C83" s="45"/>
       <c r="D83" s="48"/>
@@ -6017,7 +6017,7 @@
       <c r="L83" s="19"/>
     </row>
     <row r="84" spans="1:12" ht="30">
-      <c r="A84" s="51"/>
+      <c r="A84" s="63"/>
       <c r="B84" s="45"/>
       <c r="C84" s="45"/>
       <c r="D84" s="48"/>
@@ -6045,7 +6045,7 @@
       <c r="L84" s="19"/>
     </row>
     <row r="85" spans="1:12" ht="30">
-      <c r="A85" s="51"/>
+      <c r="A85" s="63"/>
       <c r="B85" s="45"/>
       <c r="C85" s="45"/>
       <c r="D85" s="48"/>
@@ -6073,7 +6073,7 @@
       <c r="L85" s="19"/>
     </row>
     <row r="86" spans="1:12" ht="45">
-      <c r="A86" s="51"/>
+      <c r="A86" s="63"/>
       <c r="B86" s="45"/>
       <c r="C86" s="45"/>
       <c r="D86" s="48"/>
@@ -6101,7 +6101,7 @@
       <c r="L86" s="19"/>
     </row>
     <row r="87" spans="1:12" ht="45">
-      <c r="A87" s="51"/>
+      <c r="A87" s="63"/>
       <c r="B87" s="45"/>
       <c r="C87" s="45"/>
       <c r="D87" s="48"/>
@@ -6129,7 +6129,7 @@
       <c r="L87" s="19"/>
     </row>
     <row r="88" spans="1:12" ht="45">
-      <c r="A88" s="51"/>
+      <c r="A88" s="63"/>
       <c r="B88" s="45"/>
       <c r="C88" s="45"/>
       <c r="D88" s="48"/>
@@ -6157,7 +6157,7 @@
       <c r="L88" s="19"/>
     </row>
     <row r="89" spans="1:12" ht="45">
-      <c r="A89" s="51"/>
+      <c r="A89" s="63"/>
       <c r="B89" s="45"/>
       <c r="C89" s="45"/>
       <c r="D89" s="48"/>
@@ -6185,7 +6185,7 @@
       <c r="L89" s="19"/>
     </row>
     <row r="90" spans="1:12" ht="45">
-      <c r="A90" s="51"/>
+      <c r="A90" s="63"/>
       <c r="B90" s="45"/>
       <c r="C90" s="45"/>
       <c r="D90" s="48"/>
@@ -6213,7 +6213,7 @@
       <c r="L90" s="19"/>
     </row>
     <row r="91" spans="1:12" ht="45">
-      <c r="A91" s="51"/>
+      <c r="A91" s="63"/>
       <c r="B91" s="45"/>
       <c r="C91" s="45"/>
       <c r="D91" s="48"/>
@@ -6241,7 +6241,7 @@
       <c r="L91" s="19"/>
     </row>
     <row r="92" spans="1:12" ht="45">
-      <c r="A92" s="51"/>
+      <c r="A92" s="63"/>
       <c r="B92" s="45"/>
       <c r="C92" s="45"/>
       <c r="D92" s="48"/>
@@ -6269,7 +6269,7 @@
       <c r="L92" s="19"/>
     </row>
     <row r="93" spans="1:12" ht="45">
-      <c r="A93" s="51"/>
+      <c r="A93" s="63"/>
       <c r="B93" s="45"/>
       <c r="C93" s="45"/>
       <c r="D93" s="48"/>
@@ -6297,7 +6297,7 @@
       <c r="L93" s="19"/>
     </row>
     <row r="94" spans="1:12" ht="30">
-      <c r="A94" s="51"/>
+      <c r="A94" s="63"/>
       <c r="B94" s="45"/>
       <c r="C94" s="45"/>
       <c r="D94" s="48"/>
@@ -6325,7 +6325,7 @@
       <c r="L94" s="19"/>
     </row>
     <row r="95" spans="1:12" ht="30">
-      <c r="A95" s="51"/>
+      <c r="A95" s="63"/>
       <c r="B95" s="45"/>
       <c r="C95" s="45"/>
       <c r="D95" s="48"/>
@@ -6353,7 +6353,7 @@
       <c r="L95" s="19"/>
     </row>
     <row r="96" spans="1:12" ht="30">
-      <c r="A96" s="51"/>
+      <c r="A96" s="63"/>
       <c r="B96" s="45"/>
       <c r="C96" s="45"/>
       <c r="D96" s="48"/>
@@ -6381,7 +6381,7 @@
       <c r="L96" s="19"/>
     </row>
     <row r="97" spans="1:12" ht="45">
-      <c r="A97" s="51"/>
+      <c r="A97" s="63"/>
       <c r="B97" s="45"/>
       <c r="C97" s="45"/>
       <c r="D97" s="48"/>
@@ -6409,7 +6409,7 @@
       <c r="L97" s="19"/>
     </row>
     <row r="98" spans="1:12" ht="30">
-      <c r="A98" s="51"/>
+      <c r="A98" s="63"/>
       <c r="B98" s="45"/>
       <c r="C98" s="45"/>
       <c r="D98" s="48"/>
@@ -6437,7 +6437,7 @@
       <c r="L98" s="19"/>
     </row>
     <row r="99" spans="1:12" ht="30">
-      <c r="A99" s="51"/>
+      <c r="A99" s="63"/>
       <c r="B99" s="45"/>
       <c r="C99" s="45"/>
       <c r="D99" s="48"/>
@@ -6465,7 +6465,7 @@
       <c r="L99" s="19"/>
     </row>
     <row r="100" spans="1:12" ht="30">
-      <c r="A100" s="51"/>
+      <c r="A100" s="63"/>
       <c r="B100" s="45"/>
       <c r="C100" s="45"/>
       <c r="D100" s="48"/>
@@ -6493,7 +6493,7 @@
       <c r="L100" s="19"/>
     </row>
     <row r="101" spans="1:12" ht="38.25">
-      <c r="A101" s="52"/>
+      <c r="A101" s="64"/>
       <c r="B101" s="46"/>
       <c r="C101" s="46"/>
       <c r="D101" s="49"/>
@@ -6519,16 +6519,16 @@
       <c r="L101" s="19"/>
     </row>
     <row r="102" spans="1:12" ht="45">
-      <c r="A102" s="53" t="s">
+      <c r="A102" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="B102" s="56" t="s">
+      <c r="B102" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="C102" s="56" t="s">
+      <c r="C102" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="D102" s="59" t="s">
+      <c r="D102" s="53" t="s">
         <v>640</v>
       </c>
       <c r="E102" s="37" t="s">
@@ -6555,10 +6555,10 @@
       <c r="L102" s="6"/>
     </row>
     <row r="103" spans="1:12" ht="30">
-      <c r="A103" s="54"/>
-      <c r="B103" s="57"/>
-      <c r="C103" s="57"/>
-      <c r="D103" s="60"/>
+      <c r="A103" s="57"/>
+      <c r="B103" s="60"/>
+      <c r="C103" s="60"/>
+      <c r="D103" s="54"/>
       <c r="E103" s="37" t="s">
         <v>13</v>
       </c>
@@ -6581,10 +6581,10 @@
       <c r="L103" s="6"/>
     </row>
     <row r="104" spans="1:12" ht="30">
-      <c r="A104" s="54"/>
-      <c r="B104" s="57"/>
-      <c r="C104" s="57"/>
-      <c r="D104" s="60"/>
+      <c r="A104" s="57"/>
+      <c r="B104" s="60"/>
+      <c r="C104" s="60"/>
+      <c r="D104" s="54"/>
       <c r="E104" s="37" t="s">
         <v>14</v>
       </c>
@@ -6607,10 +6607,10 @@
       <c r="L104" s="6"/>
     </row>
     <row r="105" spans="1:12" ht="30">
-      <c r="A105" s="54"/>
-      <c r="B105" s="57"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="60"/>
+      <c r="A105" s="57"/>
+      <c r="B105" s="60"/>
+      <c r="C105" s="60"/>
+      <c r="D105" s="54"/>
       <c r="E105" s="37" t="s">
         <v>15</v>
       </c>
@@ -6635,10 +6635,10 @@
       <c r="L105" s="6"/>
     </row>
     <row r="106" spans="1:12" ht="30">
-      <c r="A106" s="54"/>
-      <c r="B106" s="57"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="60"/>
+      <c r="A106" s="57"/>
+      <c r="B106" s="60"/>
+      <c r="C106" s="60"/>
+      <c r="D106" s="54"/>
       <c r="E106" s="37" t="s">
         <v>16</v>
       </c>
@@ -6663,10 +6663,10 @@
       <c r="L106" s="6"/>
     </row>
     <row r="107" spans="1:12" ht="30">
-      <c r="A107" s="54"/>
-      <c r="B107" s="57"/>
-      <c r="C107" s="57"/>
-      <c r="D107" s="60"/>
+      <c r="A107" s="57"/>
+      <c r="B107" s="60"/>
+      <c r="C107" s="60"/>
+      <c r="D107" s="54"/>
       <c r="E107" s="37" t="s">
         <v>17</v>
       </c>
@@ -6691,10 +6691,10 @@
       <c r="L107" s="6"/>
     </row>
     <row r="108" spans="1:12" ht="30">
-      <c r="A108" s="54"/>
-      <c r="B108" s="57"/>
-      <c r="C108" s="57"/>
-      <c r="D108" s="60"/>
+      <c r="A108" s="57"/>
+      <c r="B108" s="60"/>
+      <c r="C108" s="60"/>
+      <c r="D108" s="54"/>
       <c r="E108" s="37" t="s">
         <v>18</v>
       </c>
@@ -6719,10 +6719,10 @@
       <c r="L108" s="6"/>
     </row>
     <row r="109" spans="1:12" ht="30">
-      <c r="A109" s="54"/>
-      <c r="B109" s="57"/>
-      <c r="C109" s="57"/>
-      <c r="D109" s="60"/>
+      <c r="A109" s="57"/>
+      <c r="B109" s="60"/>
+      <c r="C109" s="60"/>
+      <c r="D109" s="54"/>
       <c r="E109" s="37" t="s">
         <v>19</v>
       </c>
@@ -6747,10 +6747,10 @@
       <c r="L109" s="6"/>
     </row>
     <row r="110" spans="1:12" ht="45">
-      <c r="A110" s="54"/>
-      <c r="B110" s="57"/>
-      <c r="C110" s="57"/>
-      <c r="D110" s="60"/>
+      <c r="A110" s="57"/>
+      <c r="B110" s="60"/>
+      <c r="C110" s="60"/>
+      <c r="D110" s="54"/>
       <c r="E110" s="37" t="s">
         <v>20</v>
       </c>
@@ -6775,10 +6775,10 @@
       <c r="L110" s="6"/>
     </row>
     <row r="111" spans="1:12" ht="45">
-      <c r="A111" s="54"/>
-      <c r="B111" s="57"/>
-      <c r="C111" s="57"/>
-      <c r="D111" s="60"/>
+      <c r="A111" s="57"/>
+      <c r="B111" s="60"/>
+      <c r="C111" s="60"/>
+      <c r="D111" s="54"/>
       <c r="E111" s="37" t="s">
         <v>21</v>
       </c>
@@ -6803,10 +6803,10 @@
       <c r="L111" s="6"/>
     </row>
     <row r="112" spans="1:12" ht="30">
-      <c r="A112" s="54"/>
-      <c r="B112" s="57"/>
-      <c r="C112" s="57"/>
-      <c r="D112" s="60"/>
+      <c r="A112" s="57"/>
+      <c r="B112" s="60"/>
+      <c r="C112" s="60"/>
+      <c r="D112" s="54"/>
       <c r="E112" s="37" t="s">
         <v>22</v>
       </c>
@@ -6829,10 +6829,10 @@
       <c r="L112" s="6"/>
     </row>
     <row r="113" spans="1:12" ht="30">
-      <c r="A113" s="54"/>
-      <c r="B113" s="57"/>
-      <c r="C113" s="57"/>
-      <c r="D113" s="60"/>
+      <c r="A113" s="57"/>
+      <c r="B113" s="60"/>
+      <c r="C113" s="60"/>
+      <c r="D113" s="54"/>
       <c r="E113" s="37" t="s">
         <v>23</v>
       </c>
@@ -6857,10 +6857,10 @@
       <c r="L113" s="6"/>
     </row>
     <row r="114" spans="1:12" ht="38.25">
-      <c r="A114" s="55"/>
-      <c r="B114" s="58"/>
-      <c r="C114" s="58"/>
-      <c r="D114" s="61"/>
+      <c r="A114" s="58"/>
+      <c r="B114" s="61"/>
+      <c r="C114" s="61"/>
+      <c r="D114" s="55"/>
       <c r="E114" s="37" t="s">
         <v>24</v>
       </c>
@@ -6883,7 +6883,7 @@
       <c r="L114" s="6"/>
     </row>
     <row r="115" spans="1:12" ht="45">
-      <c r="A115" s="50" t="s">
+      <c r="A115" s="62" t="s">
         <v>330</v>
       </c>
       <c r="B115" s="44" t="s">
@@ -6919,7 +6919,7 @@
       <c r="L115" s="19"/>
     </row>
     <row r="116" spans="1:12" ht="30">
-      <c r="A116" s="51"/>
+      <c r="A116" s="63"/>
       <c r="B116" s="45"/>
       <c r="C116" s="45"/>
       <c r="D116" s="48"/>
@@ -6945,7 +6945,7 @@
       <c r="L116" s="19"/>
     </row>
     <row r="117" spans="1:12" ht="45">
-      <c r="A117" s="51"/>
+      <c r="A117" s="63"/>
       <c r="B117" s="45"/>
       <c r="C117" s="45"/>
       <c r="D117" s="48"/>
@@ -6973,7 +6973,7 @@
       <c r="L117" s="19"/>
     </row>
     <row r="118" spans="1:12" ht="45">
-      <c r="A118" s="51"/>
+      <c r="A118" s="63"/>
       <c r="B118" s="45"/>
       <c r="C118" s="45"/>
       <c r="D118" s="48"/>
@@ -7001,7 +7001,7 @@
       <c r="L118" s="19"/>
     </row>
     <row r="119" spans="1:12" ht="45">
-      <c r="A119" s="51"/>
+      <c r="A119" s="63"/>
       <c r="B119" s="45"/>
       <c r="C119" s="45"/>
       <c r="D119" s="48"/>
@@ -7029,7 +7029,7 @@
       <c r="L119" s="19"/>
     </row>
     <row r="120" spans="1:12" ht="30">
-      <c r="A120" s="51"/>
+      <c r="A120" s="63"/>
       <c r="B120" s="45"/>
       <c r="C120" s="45"/>
       <c r="D120" s="48"/>
@@ -7057,7 +7057,7 @@
       <c r="L120" s="19"/>
     </row>
     <row r="121" spans="1:12" ht="30">
-      <c r="A121" s="51"/>
+      <c r="A121" s="63"/>
       <c r="B121" s="45"/>
       <c r="C121" s="45"/>
       <c r="D121" s="48"/>
@@ -7085,7 +7085,7 @@
       <c r="L121" s="19"/>
     </row>
     <row r="122" spans="1:12" ht="30">
-      <c r="A122" s="51"/>
+      <c r="A122" s="63"/>
       <c r="B122" s="45"/>
       <c r="C122" s="45"/>
       <c r="D122" s="48"/>
@@ -7113,7 +7113,7 @@
       <c r="L122" s="19"/>
     </row>
     <row r="123" spans="1:12" ht="30">
-      <c r="A123" s="51"/>
+      <c r="A123" s="63"/>
       <c r="B123" s="45"/>
       <c r="C123" s="45"/>
       <c r="D123" s="48"/>
@@ -7141,7 +7141,7 @@
       <c r="L123" s="19"/>
     </row>
     <row r="124" spans="1:12" ht="30">
-      <c r="A124" s="51"/>
+      <c r="A124" s="63"/>
       <c r="B124" s="45"/>
       <c r="C124" s="45"/>
       <c r="D124" s="48"/>
@@ -7169,7 +7169,7 @@
       <c r="L124" s="19"/>
     </row>
     <row r="125" spans="1:12" ht="30">
-      <c r="A125" s="51"/>
+      <c r="A125" s="63"/>
       <c r="B125" s="45"/>
       <c r="C125" s="45"/>
       <c r="D125" s="48"/>
@@ -7197,7 +7197,7 @@
       <c r="L125" s="19"/>
     </row>
     <row r="126" spans="1:12" ht="30">
-      <c r="A126" s="51"/>
+      <c r="A126" s="63"/>
       <c r="B126" s="45"/>
       <c r="C126" s="45"/>
       <c r="D126" s="48"/>
@@ -7225,7 +7225,7 @@
       <c r="L126" s="19"/>
     </row>
     <row r="127" spans="1:12" ht="30">
-      <c r="A127" s="51"/>
+      <c r="A127" s="63"/>
       <c r="B127" s="45"/>
       <c r="C127" s="45"/>
       <c r="D127" s="48"/>
@@ -7253,7 +7253,7 @@
       <c r="L127" s="19"/>
     </row>
     <row r="128" spans="1:12" ht="30">
-      <c r="A128" s="51"/>
+      <c r="A128" s="63"/>
       <c r="B128" s="45"/>
       <c r="C128" s="45"/>
       <c r="D128" s="48"/>
@@ -7281,7 +7281,7 @@
       <c r="L128" s="19"/>
     </row>
     <row r="129" spans="1:12" ht="30">
-      <c r="A129" s="51"/>
+      <c r="A129" s="63"/>
       <c r="B129" s="45"/>
       <c r="C129" s="45"/>
       <c r="D129" s="48"/>
@@ -7309,7 +7309,7 @@
       <c r="L129" s="19"/>
     </row>
     <row r="130" spans="1:12" ht="30">
-      <c r="A130" s="51"/>
+      <c r="A130" s="63"/>
       <c r="B130" s="45"/>
       <c r="C130" s="45"/>
       <c r="D130" s="48"/>
@@ -7337,7 +7337,7 @@
       <c r="L130" s="19"/>
     </row>
     <row r="131" spans="1:12" ht="30">
-      <c r="A131" s="51"/>
+      <c r="A131" s="63"/>
       <c r="B131" s="45"/>
       <c r="C131" s="45"/>
       <c r="D131" s="48"/>
@@ -7365,7 +7365,7 @@
       <c r="L131" s="19"/>
     </row>
     <row r="132" spans="1:12" ht="45">
-      <c r="A132" s="51"/>
+      <c r="A132" s="63"/>
       <c r="B132" s="45"/>
       <c r="C132" s="45"/>
       <c r="D132" s="48"/>
@@ -7393,7 +7393,7 @@
       <c r="L132" s="19"/>
     </row>
     <row r="133" spans="1:12" ht="45">
-      <c r="A133" s="51"/>
+      <c r="A133" s="63"/>
       <c r="B133" s="45"/>
       <c r="C133" s="45"/>
       <c r="D133" s="48"/>
@@ -7419,7 +7419,7 @@
       <c r="L133" s="19"/>
     </row>
     <row r="134" spans="1:12" ht="30">
-      <c r="A134" s="51"/>
+      <c r="A134" s="63"/>
       <c r="B134" s="45"/>
       <c r="C134" s="45"/>
       <c r="D134" s="48"/>
@@ -7447,7 +7447,7 @@
       <c r="L134" s="19"/>
     </row>
     <row r="135" spans="1:12" ht="38.25">
-      <c r="A135" s="52"/>
+      <c r="A135" s="64"/>
       <c r="B135" s="46"/>
       <c r="C135" s="46"/>
       <c r="D135" s="49"/>
@@ -7473,16 +7473,16 @@
       <c r="L135" s="19"/>
     </row>
     <row r="136" spans="1:12" ht="45">
-      <c r="A136" s="53" t="s">
+      <c r="A136" s="56" t="s">
         <v>352</v>
       </c>
-      <c r="B136" s="56" t="s">
+      <c r="B136" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="C136" s="56" t="s">
+      <c r="C136" s="59" t="s">
         <v>353</v>
       </c>
-      <c r="D136" s="59" t="s">
+      <c r="D136" s="53" t="s">
         <v>640</v>
       </c>
       <c r="E136" s="37" t="s">
@@ -7509,10 +7509,10 @@
       <c r="L136" s="6"/>
     </row>
     <row r="137" spans="1:12" ht="30">
-      <c r="A137" s="54"/>
-      <c r="B137" s="57"/>
-      <c r="C137" s="57"/>
-      <c r="D137" s="60"/>
+      <c r="A137" s="57"/>
+      <c r="B137" s="60"/>
+      <c r="C137" s="60"/>
+      <c r="D137" s="54"/>
       <c r="E137" s="37" t="s">
         <v>13</v>
       </c>
@@ -7535,10 +7535,10 @@
       <c r="L137" s="6"/>
     </row>
     <row r="138" spans="1:12" ht="30">
-      <c r="A138" s="54"/>
-      <c r="B138" s="57"/>
-      <c r="C138" s="57"/>
-      <c r="D138" s="60"/>
+      <c r="A138" s="57"/>
+      <c r="B138" s="60"/>
+      <c r="C138" s="60"/>
+      <c r="D138" s="54"/>
       <c r="E138" s="37" t="s">
         <v>14</v>
       </c>
@@ -7563,10 +7563,10 @@
       <c r="L138" s="6"/>
     </row>
     <row r="139" spans="1:12" ht="45">
-      <c r="A139" s="54"/>
-      <c r="B139" s="57"/>
-      <c r="C139" s="57"/>
-      <c r="D139" s="60"/>
+      <c r="A139" s="57"/>
+      <c r="B139" s="60"/>
+      <c r="C139" s="60"/>
+      <c r="D139" s="54"/>
       <c r="E139" s="37" t="s">
         <v>15</v>
       </c>
@@ -7589,10 +7589,10 @@
       <c r="L139" s="6"/>
     </row>
     <row r="140" spans="1:12" ht="45">
-      <c r="A140" s="54"/>
-      <c r="B140" s="57"/>
-      <c r="C140" s="57"/>
-      <c r="D140" s="60"/>
+      <c r="A140" s="57"/>
+      <c r="B140" s="60"/>
+      <c r="C140" s="60"/>
+      <c r="D140" s="54"/>
       <c r="E140" s="37" t="s">
         <v>16</v>
       </c>
@@ -7617,10 +7617,10 @@
       <c r="L140" s="6"/>
     </row>
     <row r="141" spans="1:12" ht="30">
-      <c r="A141" s="54"/>
-      <c r="B141" s="57"/>
-      <c r="C141" s="57"/>
-      <c r="D141" s="60"/>
+      <c r="A141" s="57"/>
+      <c r="B141" s="60"/>
+      <c r="C141" s="60"/>
+      <c r="D141" s="54"/>
       <c r="E141" s="37" t="s">
         <v>17</v>
       </c>
@@ -7645,10 +7645,10 @@
       <c r="L141" s="6"/>
     </row>
     <row r="142" spans="1:12" ht="30">
-      <c r="A142" s="54"/>
-      <c r="B142" s="57"/>
-      <c r="C142" s="57"/>
-      <c r="D142" s="60"/>
+      <c r="A142" s="57"/>
+      <c r="B142" s="60"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="54"/>
       <c r="E142" s="37" t="s">
         <v>18</v>
       </c>
@@ -7673,10 +7673,10 @@
       <c r="L142" s="6"/>
     </row>
     <row r="143" spans="1:12" ht="76.5">
-      <c r="A143" s="54"/>
-      <c r="B143" s="57"/>
-      <c r="C143" s="57"/>
-      <c r="D143" s="60"/>
+      <c r="A143" s="57"/>
+      <c r="B143" s="60"/>
+      <c r="C143" s="60"/>
+      <c r="D143" s="54"/>
       <c r="E143" s="37" t="s">
         <v>19</v>
       </c>
@@ -7701,10 +7701,10 @@
       <c r="L143" s="6"/>
     </row>
     <row r="144" spans="1:12" ht="30">
-      <c r="A144" s="54"/>
-      <c r="B144" s="57"/>
-      <c r="C144" s="57"/>
-      <c r="D144" s="60"/>
+      <c r="A144" s="57"/>
+      <c r="B144" s="60"/>
+      <c r="C144" s="60"/>
+      <c r="D144" s="54"/>
       <c r="E144" s="37" t="s">
         <v>20</v>
       </c>
@@ -7729,10 +7729,10 @@
       <c r="L144" s="6"/>
     </row>
     <row r="145" spans="1:12" ht="30">
-      <c r="A145" s="54"/>
-      <c r="B145" s="57"/>
-      <c r="C145" s="57"/>
-      <c r="D145" s="60"/>
+      <c r="A145" s="57"/>
+      <c r="B145" s="60"/>
+      <c r="C145" s="60"/>
+      <c r="D145" s="54"/>
       <c r="E145" s="37" t="s">
         <v>21</v>
       </c>
@@ -7757,10 +7757,10 @@
       <c r="L145" s="6"/>
     </row>
     <row r="146" spans="1:12" ht="30">
-      <c r="A146" s="54"/>
-      <c r="B146" s="57"/>
-      <c r="C146" s="57"/>
-      <c r="D146" s="60"/>
+      <c r="A146" s="57"/>
+      <c r="B146" s="60"/>
+      <c r="C146" s="60"/>
+      <c r="D146" s="54"/>
       <c r="E146" s="37" t="s">
         <v>22</v>
       </c>
@@ -7785,10 +7785,10 @@
       <c r="L146" s="6"/>
     </row>
     <row r="147" spans="1:12" ht="30">
-      <c r="A147" s="54"/>
-      <c r="B147" s="57"/>
-      <c r="C147" s="57"/>
-      <c r="D147" s="60"/>
+      <c r="A147" s="57"/>
+      <c r="B147" s="60"/>
+      <c r="C147" s="60"/>
+      <c r="D147" s="54"/>
       <c r="E147" s="37" t="s">
         <v>23</v>
       </c>
@@ -7813,10 +7813,10 @@
       <c r="L147" s="6"/>
     </row>
     <row r="148" spans="1:12" ht="30">
-      <c r="A148" s="54"/>
-      <c r="B148" s="57"/>
-      <c r="C148" s="57"/>
-      <c r="D148" s="60"/>
+      <c r="A148" s="57"/>
+      <c r="B148" s="60"/>
+      <c r="C148" s="60"/>
+      <c r="D148" s="54"/>
       <c r="E148" s="37" t="s">
         <v>24</v>
       </c>
@@ -7841,10 +7841,10 @@
       <c r="L148" s="6"/>
     </row>
     <row r="149" spans="1:12" ht="30">
-      <c r="A149" s="54"/>
-      <c r="B149" s="57"/>
-      <c r="C149" s="57"/>
-      <c r="D149" s="60"/>
+      <c r="A149" s="57"/>
+      <c r="B149" s="60"/>
+      <c r="C149" s="60"/>
+      <c r="D149" s="54"/>
       <c r="E149" s="37" t="s">
         <v>25</v>
       </c>
@@ -7869,10 +7869,10 @@
       <c r="L149" s="6"/>
     </row>
     <row r="150" spans="1:12" ht="45">
-      <c r="A150" s="54"/>
-      <c r="B150" s="57"/>
-      <c r="C150" s="57"/>
-      <c r="D150" s="60"/>
+      <c r="A150" s="57"/>
+      <c r="B150" s="60"/>
+      <c r="C150" s="60"/>
+      <c r="D150" s="54"/>
       <c r="E150" s="37" t="s">
         <v>54</v>
       </c>
@@ -7897,10 +7897,10 @@
       <c r="L150" s="6"/>
     </row>
     <row r="151" spans="1:12" ht="30">
-      <c r="A151" s="54"/>
-      <c r="B151" s="57"/>
-      <c r="C151" s="57"/>
-      <c r="D151" s="60"/>
+      <c r="A151" s="57"/>
+      <c r="B151" s="60"/>
+      <c r="C151" s="60"/>
+      <c r="D151" s="54"/>
       <c r="E151" s="37" t="s">
         <v>143</v>
       </c>
@@ -7925,10 +7925,10 @@
       <c r="L151" s="6"/>
     </row>
     <row r="152" spans="1:12" ht="30">
-      <c r="A152" s="54"/>
-      <c r="B152" s="57"/>
-      <c r="C152" s="57"/>
-      <c r="D152" s="60"/>
+      <c r="A152" s="57"/>
+      <c r="B152" s="60"/>
+      <c r="C152" s="60"/>
+      <c r="D152" s="54"/>
       <c r="E152" s="37" t="s">
         <v>165</v>
       </c>
@@ -7953,10 +7953,10 @@
       <c r="L152" s="6"/>
     </row>
     <row r="153" spans="1:12" ht="45">
-      <c r="A153" s="54"/>
-      <c r="B153" s="57"/>
-      <c r="C153" s="57"/>
-      <c r="D153" s="60"/>
+      <c r="A153" s="57"/>
+      <c r="B153" s="60"/>
+      <c r="C153" s="60"/>
+      <c r="D153" s="54"/>
       <c r="E153" s="37" t="s">
         <v>166</v>
       </c>
@@ -7981,10 +7981,10 @@
       <c r="L153" s="6"/>
     </row>
     <row r="154" spans="1:12" ht="45">
-      <c r="A154" s="54"/>
-      <c r="B154" s="57"/>
-      <c r="C154" s="57"/>
-      <c r="D154" s="60"/>
+      <c r="A154" s="57"/>
+      <c r="B154" s="60"/>
+      <c r="C154" s="60"/>
+      <c r="D154" s="54"/>
       <c r="E154" s="37" t="s">
         <v>167</v>
       </c>
@@ -8009,10 +8009,10 @@
       <c r="L154" s="6"/>
     </row>
     <row r="155" spans="1:12" ht="30">
-      <c r="A155" s="54"/>
-      <c r="B155" s="57"/>
-      <c r="C155" s="57"/>
-      <c r="D155" s="60"/>
+      <c r="A155" s="57"/>
+      <c r="B155" s="60"/>
+      <c r="C155" s="60"/>
+      <c r="D155" s="54"/>
       <c r="E155" s="37" t="s">
         <v>168</v>
       </c>
@@ -8037,10 +8037,10 @@
       <c r="L155" s="6"/>
     </row>
     <row r="156" spans="1:12" ht="45">
-      <c r="A156" s="54"/>
-      <c r="B156" s="57"/>
-      <c r="C156" s="57"/>
-      <c r="D156" s="60"/>
+      <c r="A156" s="57"/>
+      <c r="B156" s="60"/>
+      <c r="C156" s="60"/>
+      <c r="D156" s="54"/>
       <c r="E156" s="37" t="s">
         <v>177</v>
       </c>
@@ -8065,10 +8065,10 @@
       <c r="L156" s="6"/>
     </row>
     <row r="157" spans="1:12" ht="30">
-      <c r="A157" s="54"/>
-      <c r="B157" s="57"/>
-      <c r="C157" s="57"/>
-      <c r="D157" s="60"/>
+      <c r="A157" s="57"/>
+      <c r="B157" s="60"/>
+      <c r="C157" s="60"/>
+      <c r="D157" s="54"/>
       <c r="E157" s="37" t="s">
         <v>178</v>
       </c>
@@ -8093,10 +8093,10 @@
       <c r="L157" s="6"/>
     </row>
     <row r="158" spans="1:12" ht="30">
-      <c r="A158" s="54"/>
-      <c r="B158" s="57"/>
-      <c r="C158" s="57"/>
-      <c r="D158" s="60"/>
+      <c r="A158" s="57"/>
+      <c r="B158" s="60"/>
+      <c r="C158" s="60"/>
+      <c r="D158" s="54"/>
       <c r="E158" s="37" t="s">
         <v>179</v>
       </c>
@@ -8121,10 +8121,10 @@
       <c r="L158" s="6"/>
     </row>
     <row r="159" spans="1:12" ht="30">
-      <c r="A159" s="54"/>
-      <c r="B159" s="57"/>
-      <c r="C159" s="57"/>
-      <c r="D159" s="60"/>
+      <c r="A159" s="57"/>
+      <c r="B159" s="60"/>
+      <c r="C159" s="60"/>
+      <c r="D159" s="54"/>
       <c r="E159" s="37" t="s">
         <v>183</v>
       </c>
@@ -8149,10 +8149,10 @@
       <c r="L159" s="6"/>
     </row>
     <row r="160" spans="1:12" ht="30">
-      <c r="A160" s="54"/>
-      <c r="B160" s="57"/>
-      <c r="C160" s="57"/>
-      <c r="D160" s="60"/>
+      <c r="A160" s="57"/>
+      <c r="B160" s="60"/>
+      <c r="C160" s="60"/>
+      <c r="D160" s="54"/>
       <c r="E160" s="37" t="s">
         <v>184</v>
       </c>
@@ -8177,10 +8177,10 @@
       <c r="L160" s="6"/>
     </row>
     <row r="161" spans="1:12" ht="30">
-      <c r="A161" s="54"/>
-      <c r="B161" s="57"/>
-      <c r="C161" s="57"/>
-      <c r="D161" s="60"/>
+      <c r="A161" s="57"/>
+      <c r="B161" s="60"/>
+      <c r="C161" s="60"/>
+      <c r="D161" s="54"/>
       <c r="E161" s="37" t="s">
         <v>185</v>
       </c>
@@ -8205,10 +8205,10 @@
       <c r="L161" s="6"/>
     </row>
     <row r="162" spans="1:12" ht="30">
-      <c r="A162" s="54"/>
-      <c r="B162" s="57"/>
-      <c r="C162" s="57"/>
-      <c r="D162" s="60"/>
+      <c r="A162" s="57"/>
+      <c r="B162" s="60"/>
+      <c r="C162" s="60"/>
+      <c r="D162" s="54"/>
       <c r="E162" s="37" t="s">
         <v>419</v>
       </c>
@@ -8233,10 +8233,10 @@
       <c r="L162" s="6"/>
     </row>
     <row r="163" spans="1:12" ht="30">
-      <c r="A163" s="54"/>
-      <c r="B163" s="57"/>
-      <c r="C163" s="57"/>
-      <c r="D163" s="60"/>
+      <c r="A163" s="57"/>
+      <c r="B163" s="60"/>
+      <c r="C163" s="60"/>
+      <c r="D163" s="54"/>
       <c r="E163" s="37" t="s">
         <v>420</v>
       </c>
@@ -8261,10 +8261,10 @@
       <c r="L163" s="6"/>
     </row>
     <row r="164" spans="1:12" ht="30">
-      <c r="A164" s="54"/>
-      <c r="B164" s="57"/>
-      <c r="C164" s="57"/>
-      <c r="D164" s="60"/>
+      <c r="A164" s="57"/>
+      <c r="B164" s="60"/>
+      <c r="C164" s="60"/>
+      <c r="D164" s="54"/>
       <c r="E164" s="37" t="s">
         <v>421</v>
       </c>
@@ -8289,10 +8289,10 @@
       <c r="L164" s="6"/>
     </row>
     <row r="165" spans="1:12" ht="30">
-      <c r="A165" s="54"/>
-      <c r="B165" s="57"/>
-      <c r="C165" s="57"/>
-      <c r="D165" s="60"/>
+      <c r="A165" s="57"/>
+      <c r="B165" s="60"/>
+      <c r="C165" s="60"/>
+      <c r="D165" s="54"/>
       <c r="E165" s="37" t="s">
         <v>422</v>
       </c>
@@ -8317,10 +8317,10 @@
       <c r="L165" s="6"/>
     </row>
     <row r="166" spans="1:12" ht="45">
-      <c r="A166" s="54"/>
-      <c r="B166" s="57"/>
-      <c r="C166" s="57"/>
-      <c r="D166" s="60"/>
+      <c r="A166" s="57"/>
+      <c r="B166" s="60"/>
+      <c r="C166" s="60"/>
+      <c r="D166" s="54"/>
       <c r="E166" s="37" t="s">
         <v>423</v>
       </c>
@@ -8345,10 +8345,10 @@
       <c r="L166" s="6"/>
     </row>
     <row r="167" spans="1:12" ht="45">
-      <c r="A167" s="54"/>
-      <c r="B167" s="57"/>
-      <c r="C167" s="57"/>
-      <c r="D167" s="60"/>
+      <c r="A167" s="57"/>
+      <c r="B167" s="60"/>
+      <c r="C167" s="60"/>
+      <c r="D167" s="54"/>
       <c r="E167" s="37" t="s">
         <v>424</v>
       </c>
@@ -8373,10 +8373,10 @@
       <c r="L167" s="6"/>
     </row>
     <row r="168" spans="1:12" ht="45">
-      <c r="A168" s="54"/>
-      <c r="B168" s="57"/>
-      <c r="C168" s="57"/>
-      <c r="D168" s="60"/>
+      <c r="A168" s="57"/>
+      <c r="B168" s="60"/>
+      <c r="C168" s="60"/>
+      <c r="D168" s="54"/>
       <c r="E168" s="37" t="s">
         <v>425</v>
       </c>
@@ -8401,10 +8401,10 @@
       <c r="L168" s="6"/>
     </row>
     <row r="169" spans="1:12" ht="45">
-      <c r="A169" s="54"/>
-      <c r="B169" s="57"/>
-      <c r="C169" s="57"/>
-      <c r="D169" s="60"/>
+      <c r="A169" s="57"/>
+      <c r="B169" s="60"/>
+      <c r="C169" s="60"/>
+      <c r="D169" s="54"/>
       <c r="E169" s="37" t="s">
         <v>426</v>
       </c>
@@ -8429,10 +8429,10 @@
       <c r="L169" s="6"/>
     </row>
     <row r="170" spans="1:12" ht="30">
-      <c r="A170" s="54"/>
-      <c r="B170" s="57"/>
-      <c r="C170" s="57"/>
-      <c r="D170" s="60"/>
+      <c r="A170" s="57"/>
+      <c r="B170" s="60"/>
+      <c r="C170" s="60"/>
+      <c r="D170" s="54"/>
       <c r="E170" s="37" t="s">
         <v>427</v>
       </c>
@@ -8457,10 +8457,10 @@
       <c r="L170" s="6"/>
     </row>
     <row r="171" spans="1:12" ht="30">
-      <c r="A171" s="54"/>
-      <c r="B171" s="57"/>
-      <c r="C171" s="57"/>
-      <c r="D171" s="60"/>
+      <c r="A171" s="57"/>
+      <c r="B171" s="60"/>
+      <c r="C171" s="60"/>
+      <c r="D171" s="54"/>
       <c r="E171" s="37" t="s">
         <v>428</v>
       </c>
@@ -8485,10 +8485,10 @@
       <c r="L171" s="6"/>
     </row>
     <row r="172" spans="1:12" ht="30">
-      <c r="A172" s="54"/>
-      <c r="B172" s="57"/>
-      <c r="C172" s="57"/>
-      <c r="D172" s="60"/>
+      <c r="A172" s="57"/>
+      <c r="B172" s="60"/>
+      <c r="C172" s="60"/>
+      <c r="D172" s="54"/>
       <c r="E172" s="37" t="s">
         <v>429</v>
       </c>
@@ -8513,10 +8513,10 @@
       <c r="L172" s="6"/>
     </row>
     <row r="173" spans="1:12" ht="45">
-      <c r="A173" s="54"/>
-      <c r="B173" s="57"/>
-      <c r="C173" s="57"/>
-      <c r="D173" s="60"/>
+      <c r="A173" s="57"/>
+      <c r="B173" s="60"/>
+      <c r="C173" s="60"/>
+      <c r="D173" s="54"/>
       <c r="E173" s="37" t="s">
         <v>430</v>
       </c>
@@ -8541,10 +8541,10 @@
       <c r="L173" s="6"/>
     </row>
     <row r="174" spans="1:12" ht="60">
-      <c r="A174" s="54"/>
-      <c r="B174" s="57"/>
-      <c r="C174" s="57"/>
-      <c r="D174" s="60"/>
+      <c r="A174" s="57"/>
+      <c r="B174" s="60"/>
+      <c r="C174" s="60"/>
+      <c r="D174" s="54"/>
       <c r="E174" s="37" t="s">
         <v>431</v>
       </c>
@@ -8569,10 +8569,10 @@
       <c r="L174" s="6"/>
     </row>
     <row r="175" spans="1:12" ht="30">
-      <c r="A175" s="54"/>
-      <c r="B175" s="57"/>
-      <c r="C175" s="57"/>
-      <c r="D175" s="60"/>
+      <c r="A175" s="57"/>
+      <c r="B175" s="60"/>
+      <c r="C175" s="60"/>
+      <c r="D175" s="54"/>
       <c r="E175" s="37" t="s">
         <v>432</v>
       </c>
@@ -8597,10 +8597,10 @@
       <c r="L175" s="6"/>
     </row>
     <row r="176" spans="1:12" ht="30">
-      <c r="A176" s="54"/>
-      <c r="B176" s="57"/>
-      <c r="C176" s="57"/>
-      <c r="D176" s="60"/>
+      <c r="A176" s="57"/>
+      <c r="B176" s="60"/>
+      <c r="C176" s="60"/>
+      <c r="D176" s="54"/>
       <c r="E176" s="37" t="s">
         <v>433</v>
       </c>
@@ -8625,10 +8625,10 @@
       <c r="L176" s="6"/>
     </row>
     <row r="177" spans="1:12" ht="30">
-      <c r="A177" s="54"/>
-      <c r="B177" s="57"/>
-      <c r="C177" s="57"/>
-      <c r="D177" s="60"/>
+      <c r="A177" s="57"/>
+      <c r="B177" s="60"/>
+      <c r="C177" s="60"/>
+      <c r="D177" s="54"/>
       <c r="E177" s="37" t="s">
         <v>434</v>
       </c>
@@ -8653,10 +8653,10 @@
       <c r="L177" s="6"/>
     </row>
     <row r="178" spans="1:12" ht="30">
-      <c r="A178" s="54"/>
-      <c r="B178" s="57"/>
-      <c r="C178" s="57"/>
-      <c r="D178" s="60"/>
+      <c r="A178" s="57"/>
+      <c r="B178" s="60"/>
+      <c r="C178" s="60"/>
+      <c r="D178" s="54"/>
       <c r="E178" s="37" t="s">
         <v>435</v>
       </c>
@@ -8681,10 +8681,10 @@
       <c r="L178" s="6"/>
     </row>
     <row r="179" spans="1:12" ht="30">
-      <c r="A179" s="54"/>
-      <c r="B179" s="57"/>
-      <c r="C179" s="57"/>
-      <c r="D179" s="60"/>
+      <c r="A179" s="57"/>
+      <c r="B179" s="60"/>
+      <c r="C179" s="60"/>
+      <c r="D179" s="54"/>
       <c r="E179" s="37" t="s">
         <v>499</v>
       </c>
@@ -8709,10 +8709,10 @@
       <c r="L179" s="6"/>
     </row>
     <row r="180" spans="1:12" ht="30">
-      <c r="A180" s="54"/>
-      <c r="B180" s="57"/>
-      <c r="C180" s="57"/>
-      <c r="D180" s="60"/>
+      <c r="A180" s="57"/>
+      <c r="B180" s="60"/>
+      <c r="C180" s="60"/>
+      <c r="D180" s="54"/>
       <c r="E180" s="37" t="s">
         <v>500</v>
       </c>
@@ -8737,10 +8737,10 @@
       <c r="L180" s="6"/>
     </row>
     <row r="181" spans="1:12" ht="45">
-      <c r="A181" s="54"/>
-      <c r="B181" s="57"/>
-      <c r="C181" s="57"/>
-      <c r="D181" s="60"/>
+      <c r="A181" s="57"/>
+      <c r="B181" s="60"/>
+      <c r="C181" s="60"/>
+      <c r="D181" s="54"/>
       <c r="E181" s="37" t="s">
         <v>501</v>
       </c>
@@ -8765,10 +8765,10 @@
       <c r="L181" s="6"/>
     </row>
     <row r="182" spans="1:12" ht="45">
-      <c r="A182" s="54"/>
-      <c r="B182" s="57"/>
-      <c r="C182" s="57"/>
-      <c r="D182" s="60"/>
+      <c r="A182" s="57"/>
+      <c r="B182" s="60"/>
+      <c r="C182" s="60"/>
+      <c r="D182" s="54"/>
       <c r="E182" s="37" t="s">
         <v>744</v>
       </c>
@@ -8793,10 +8793,10 @@
       <c r="L182" s="6"/>
     </row>
     <row r="183" spans="1:12" ht="30">
-      <c r="A183" s="54"/>
-      <c r="B183" s="57"/>
-      <c r="C183" s="57"/>
-      <c r="D183" s="60"/>
+      <c r="A183" s="57"/>
+      <c r="B183" s="60"/>
+      <c r="C183" s="60"/>
+      <c r="D183" s="54"/>
       <c r="E183" s="37" t="s">
         <v>764</v>
       </c>
@@ -8821,10 +8821,10 @@
       <c r="L183" s="6"/>
     </row>
     <row r="184" spans="1:12" ht="38.25">
-      <c r="A184" s="55"/>
-      <c r="B184" s="58"/>
-      <c r="C184" s="58"/>
-      <c r="D184" s="61"/>
+      <c r="A184" s="58"/>
+      <c r="B184" s="61"/>
+      <c r="C184" s="61"/>
+      <c r="D184" s="55"/>
       <c r="E184" s="37" t="s">
         <v>784</v>
       </c>
@@ -8848,6 +8848,38 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A115:A135"/>
+    <mergeCell ref="B115:B135"/>
+    <mergeCell ref="C115:C135"/>
+    <mergeCell ref="D115:D135"/>
+    <mergeCell ref="A136:A184"/>
+    <mergeCell ref="B136:B184"/>
+    <mergeCell ref="C136:C184"/>
+    <mergeCell ref="D136:D184"/>
+    <mergeCell ref="A77:A101"/>
+    <mergeCell ref="B77:B101"/>
+    <mergeCell ref="C77:C101"/>
+    <mergeCell ref="D77:D101"/>
+    <mergeCell ref="A102:A114"/>
+    <mergeCell ref="B102:B114"/>
+    <mergeCell ref="C102:C114"/>
+    <mergeCell ref="D102:D114"/>
+    <mergeCell ref="A59:A65"/>
+    <mergeCell ref="B59:B65"/>
+    <mergeCell ref="C59:C65"/>
+    <mergeCell ref="D59:D65"/>
+    <mergeCell ref="A66:A76"/>
+    <mergeCell ref="B66:B76"/>
+    <mergeCell ref="C66:C76"/>
+    <mergeCell ref="D66:D76"/>
+    <mergeCell ref="A31:A46"/>
+    <mergeCell ref="B31:B46"/>
+    <mergeCell ref="C31:C46"/>
+    <mergeCell ref="D31:D46"/>
+    <mergeCell ref="A47:A58"/>
+    <mergeCell ref="B47:B58"/>
+    <mergeCell ref="C47:C58"/>
+    <mergeCell ref="D47:D58"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C2:C17"/>
@@ -8856,38 +8888,6 @@
     <mergeCell ref="B18:B30"/>
     <mergeCell ref="C18:C30"/>
     <mergeCell ref="D18:D30"/>
-    <mergeCell ref="A31:A46"/>
-    <mergeCell ref="B31:B46"/>
-    <mergeCell ref="C31:C46"/>
-    <mergeCell ref="D31:D46"/>
-    <mergeCell ref="A47:A58"/>
-    <mergeCell ref="B47:B58"/>
-    <mergeCell ref="C47:C58"/>
-    <mergeCell ref="D47:D58"/>
-    <mergeCell ref="A59:A65"/>
-    <mergeCell ref="B59:B65"/>
-    <mergeCell ref="C59:C65"/>
-    <mergeCell ref="D59:D65"/>
-    <mergeCell ref="A66:A76"/>
-    <mergeCell ref="B66:B76"/>
-    <mergeCell ref="C66:C76"/>
-    <mergeCell ref="D66:D76"/>
-    <mergeCell ref="A77:A101"/>
-    <mergeCell ref="B77:B101"/>
-    <mergeCell ref="C77:C101"/>
-    <mergeCell ref="D77:D101"/>
-    <mergeCell ref="A102:A114"/>
-    <mergeCell ref="B102:B114"/>
-    <mergeCell ref="C102:C114"/>
-    <mergeCell ref="D102:D114"/>
-    <mergeCell ref="A115:A135"/>
-    <mergeCell ref="B115:B135"/>
-    <mergeCell ref="C115:C135"/>
-    <mergeCell ref="D115:D135"/>
-    <mergeCell ref="A136:A184"/>
-    <mergeCell ref="B136:B184"/>
-    <mergeCell ref="C136:C184"/>
-    <mergeCell ref="D136:D184"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G36" r:id="rId1"/>

</xml_diff>